<commit_message>
問い合わせ履歴，随時対応 Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/テストケース.xlsx
+++ b/テストケース.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD31D323-A869-4543-874D-056C9E744FE6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14810" windowHeight="8000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14805" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="001_物件管理" sheetId="1" r:id="rId1"/>
@@ -14,7 +13,7 @@
     <sheet name="備考1" sheetId="2" r:id="rId4"/>
     <sheet name="備考2" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -2097,18 +2096,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -2116,14 +2115,14 @@
     <font>
       <sz val="10"/>
       <color theme="0"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -2131,7 +2130,7 @@
     <font>
       <sz val="10"/>
       <color theme="0"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -2331,7 +2330,7 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -2366,7 +2365,7 @@
         <xdr:cNvPr id="3" name="図 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6541EA01-6FAB-48A4-A7B7-7B82327644E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6541EA01-6FAB-48A4-A7B7-7B82327644E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2375,10 +2374,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2421,7 +2420,7 @@
         <xdr:cNvPr id="3" name="図 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E3E2872-674B-4C30-9DBA-BFEFBCA09095}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E3E2872-674B-4C30-9DBA-BFEFBCA09095}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2430,10 +2429,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2457,7 +2456,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2499,7 +2498,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2531,27 +2530,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2583,24 +2564,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2776,17 +2739,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:BT41"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6328125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="16384" width="2.6328125" style="1"/>
+    <col min="1" max="16384" width="2.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:72">
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2850,7 +2815,7 @@
       <c r="AX2" s="3"/>
       <c r="AY2" s="4"/>
     </row>
-    <row r="3" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:72">
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
@@ -2914,7 +2879,7 @@
       <c r="AX3" s="12"/>
       <c r="AY3" s="13"/>
     </row>
-    <row r="5" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:72">
       <c r="B5" s="22" t="s">
         <v>21</v>
       </c>
@@ -3001,7 +2966,7 @@
       </c>
       <c r="BT5" s="18"/>
     </row>
-    <row r="6" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:72">
       <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
@@ -3051,7 +3016,7 @@
       <c r="BS6" s="20"/>
       <c r="BT6" s="21"/>
     </row>
-    <row r="7" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:72">
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
@@ -3099,7 +3064,7 @@
       <c r="BS7" s="20"/>
       <c r="BT7" s="21"/>
     </row>
-    <row r="8" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:72">
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
@@ -3171,7 +3136,7 @@
       <c r="BS8" s="20"/>
       <c r="BT8" s="21"/>
     </row>
-    <row r="9" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:72">
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
@@ -3254,7 +3219,7 @@
       <c r="BS9" s="20"/>
       <c r="BT9" s="21"/>
     </row>
-    <row r="10" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:72">
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
@@ -3338,7 +3303,7 @@
       <c r="BS10" s="20"/>
       <c r="BT10" s="21"/>
     </row>
-    <row r="11" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:72">
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
@@ -3422,7 +3387,7 @@
       <c r="BS11" s="20"/>
       <c r="BT11" s="21"/>
     </row>
-    <row r="12" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:72">
       <c r="B12" s="14"/>
       <c r="C12" s="15"/>
       <c r="D12" s="16"/>
@@ -3506,7 +3471,7 @@
       <c r="BS12" s="20"/>
       <c r="BT12" s="21"/>
     </row>
-    <row r="13" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:72">
       <c r="B13" s="14"/>
       <c r="C13" s="15"/>
       <c r="D13" s="16"/>
@@ -3590,7 +3555,7 @@
       <c r="BS13" s="20"/>
       <c r="BT13" s="21"/>
     </row>
-    <row r="14" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:72">
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
@@ -3674,7 +3639,7 @@
       <c r="BS14" s="20"/>
       <c r="BT14" s="21"/>
     </row>
-    <row r="15" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:72">
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
       <c r="D15" s="16"/>
@@ -3745,7 +3710,7 @@
       <c r="BS15" s="20"/>
       <c r="BT15" s="21"/>
     </row>
-    <row r="16" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:72">
       <c r="B16" s="14"/>
       <c r="C16" s="15"/>
       <c r="D16" s="16"/>
@@ -3816,7 +3781,7 @@
       <c r="BS16" s="20"/>
       <c r="BT16" s="21"/>
     </row>
-    <row r="17" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:72">
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
       <c r="D17" s="16"/>
@@ -3900,7 +3865,7 @@
       <c r="BS17" s="20"/>
       <c r="BT17" s="21"/>
     </row>
-    <row r="18" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:72">
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="16"/>
@@ -3982,7 +3947,7 @@
       <c r="BS18" s="20"/>
       <c r="BT18" s="21"/>
     </row>
-    <row r="19" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:72">
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
       <c r="D19" s="16"/>
@@ -4058,7 +4023,7 @@
       <c r="BS19" s="20"/>
       <c r="BT19" s="21"/>
     </row>
-    <row r="20" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:72">
       <c r="B20" s="14"/>
       <c r="C20" s="15"/>
       <c r="D20" s="16"/>
@@ -4134,7 +4099,7 @@
       <c r="BS20" s="20"/>
       <c r="BT20" s="21"/>
     </row>
-    <row r="21" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:72">
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16"/>
@@ -4210,7 +4175,7 @@
       <c r="BS21" s="20"/>
       <c r="BT21" s="21"/>
     </row>
-    <row r="22" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:72">
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
       <c r="D22" s="16"/>
@@ -4286,7 +4251,7 @@
       <c r="BS22" s="20"/>
       <c r="BT22" s="21"/>
     </row>
-    <row r="23" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:72">
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
       <c r="D23" s="16"/>
@@ -4362,7 +4327,7 @@
       <c r="BS23" s="20"/>
       <c r="BT23" s="21"/>
     </row>
-    <row r="24" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:72">
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
       <c r="D24" s="16"/>
@@ -4438,7 +4403,7 @@
       <c r="BS24" s="20"/>
       <c r="BT24" s="21"/>
     </row>
-    <row r="25" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:72">
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
       <c r="D25" s="16"/>
@@ -4514,7 +4479,7 @@
       <c r="BS25" s="20"/>
       <c r="BT25" s="21"/>
     </row>
-    <row r="26" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:72">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="16"/>
@@ -4590,7 +4555,7 @@
       <c r="BS26" s="20"/>
       <c r="BT26" s="21"/>
     </row>
-    <row r="27" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:72">
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
       <c r="D27" s="16"/>
@@ -4666,7 +4631,7 @@
       <c r="BS27" s="20"/>
       <c r="BT27" s="21"/>
     </row>
-    <row r="28" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:72">
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
       <c r="D28" s="16"/>
@@ -4742,7 +4707,7 @@
       <c r="BS28" s="20"/>
       <c r="BT28" s="21"/>
     </row>
-    <row r="29" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:72">
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
       <c r="D29" s="16"/>
@@ -4818,7 +4783,7 @@
       <c r="BS29" s="20"/>
       <c r="BT29" s="21"/>
     </row>
-    <row r="30" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:72">
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
       <c r="D30" s="16"/>
@@ -4894,7 +4859,7 @@
       <c r="BS30" s="20"/>
       <c r="BT30" s="21"/>
     </row>
-    <row r="31" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:72">
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
       <c r="D31" s="16"/>
@@ -4970,7 +4935,7 @@
       <c r="BS31" s="20"/>
       <c r="BT31" s="21"/>
     </row>
-    <row r="32" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:72">
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
       <c r="D32" s="16"/>
@@ -5046,7 +5011,7 @@
       <c r="BS32" s="20"/>
       <c r="BT32" s="21"/>
     </row>
-    <row r="33" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:72">
       <c r="B33" s="14"/>
       <c r="C33" s="15"/>
       <c r="D33" s="16"/>
@@ -5122,7 +5087,7 @@
       <c r="BS33" s="20"/>
       <c r="BT33" s="21"/>
     </row>
-    <row r="34" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:72">
       <c r="B34" s="14"/>
       <c r="C34" s="15"/>
       <c r="D34" s="16"/>
@@ -5198,7 +5163,7 @@
       <c r="BS34" s="20"/>
       <c r="BT34" s="21"/>
     </row>
-    <row r="35" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:72">
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
       <c r="D35" s="16"/>
@@ -5274,7 +5239,7 @@
       <c r="BS35" s="20"/>
       <c r="BT35" s="21"/>
     </row>
-    <row r="36" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:72">
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
       <c r="D36" s="16"/>
@@ -5350,7 +5315,7 @@
       <c r="BS36" s="20"/>
       <c r="BT36" s="21"/>
     </row>
-    <row r="37" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:72">
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
       <c r="D37" s="16"/>
@@ -5426,7 +5391,7 @@
       <c r="BS37" s="20"/>
       <c r="BT37" s="21"/>
     </row>
-    <row r="38" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:72">
       <c r="B38" s="14"/>
       <c r="C38" s="15"/>
       <c r="D38" s="16"/>
@@ -5502,7 +5467,7 @@
       <c r="BS38" s="20"/>
       <c r="BT38" s="21"/>
     </row>
-    <row r="39" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:72">
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
       <c r="D39" s="16"/>
@@ -5578,7 +5543,7 @@
       <c r="BS39" s="20"/>
       <c r="BT39" s="21"/>
     </row>
-    <row r="40" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:72">
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
       <c r="D40" s="16"/>
@@ -5654,7 +5619,7 @@
       <c r="BS40" s="20"/>
       <c r="BT40" s="21"/>
     </row>
-    <row r="41" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:72">
       <c r="B41" s="14"/>
       <c r="C41" s="15"/>
       <c r="D41" s="16"/>
@@ -5738,19 +5703,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:BT41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U34" sqref="U34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6328125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="16384" width="2.6328125" style="1"/>
+    <col min="1" max="16384" width="2.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:72">
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
@@ -5814,7 +5779,7 @@
       <c r="AX2" s="3"/>
       <c r="AY2" s="4"/>
     </row>
-    <row r="3" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:72">
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
@@ -5878,7 +5843,7 @@
       <c r="AX3" s="12"/>
       <c r="AY3" s="13"/>
     </row>
-    <row r="5" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:72">
       <c r="B5" s="22" t="s">
         <v>21</v>
       </c>
@@ -5965,7 +5930,7 @@
       </c>
       <c r="BT5" s="18"/>
     </row>
-    <row r="6" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:72">
       <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
@@ -6015,7 +5980,7 @@
       <c r="BS6" s="20"/>
       <c r="BT6" s="21"/>
     </row>
-    <row r="7" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:72">
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
@@ -6063,7 +6028,7 @@
       <c r="BS7" s="20"/>
       <c r="BT7" s="21"/>
     </row>
-    <row r="8" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:72">
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
@@ -6121,7 +6086,7 @@
       <c r="BS8" s="20"/>
       <c r="BT8" s="21"/>
     </row>
-    <row r="9" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:72">
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
@@ -6202,7 +6167,7 @@
       <c r="BS9" s="20"/>
       <c r="BT9" s="21"/>
     </row>
-    <row r="10" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:72">
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
@@ -6286,7 +6251,7 @@
       <c r="BS10" s="20"/>
       <c r="BT10" s="21"/>
     </row>
-    <row r="11" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:72">
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
@@ -6359,7 +6324,7 @@
       <c r="BS11" s="20"/>
       <c r="BT11" s="21"/>
     </row>
-    <row r="12" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:72">
       <c r="B12" s="14"/>
       <c r="C12" s="15"/>
       <c r="D12" s="16"/>
@@ -6441,7 +6406,7 @@
       <c r="BS12" s="20"/>
       <c r="BT12" s="21"/>
     </row>
-    <row r="13" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:72">
       <c r="B13" s="14"/>
       <c r="C13" s="15"/>
       <c r="D13" s="16"/>
@@ -6525,7 +6490,7 @@
       <c r="BS13" s="20"/>
       <c r="BT13" s="21"/>
     </row>
-    <row r="14" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:72">
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
@@ -6607,7 +6572,7 @@
       <c r="BS14" s="20"/>
       <c r="BT14" s="21"/>
     </row>
-    <row r="15" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:72">
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
       <c r="D15" s="16"/>
@@ -6681,7 +6646,7 @@
       <c r="BS15" s="20"/>
       <c r="BT15" s="21"/>
     </row>
-    <row r="16" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:72">
       <c r="B16" s="14"/>
       <c r="C16" s="15"/>
       <c r="D16" s="16"/>
@@ -6752,7 +6717,7 @@
       <c r="BS16" s="20"/>
       <c r="BT16" s="21"/>
     </row>
-    <row r="17" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:72">
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
       <c r="D17" s="16"/>
@@ -6836,7 +6801,7 @@
       <c r="BS17" s="20"/>
       <c r="BT17" s="21"/>
     </row>
-    <row r="18" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:72">
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="16"/>
@@ -6918,7 +6883,7 @@
       <c r="BS18" s="20"/>
       <c r="BT18" s="21"/>
     </row>
-    <row r="19" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:72">
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
       <c r="D19" s="16"/>
@@ -7000,7 +6965,7 @@
       <c r="BS19" s="20"/>
       <c r="BT19" s="21"/>
     </row>
-    <row r="20" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:72">
       <c r="B20" s="14"/>
       <c r="C20" s="15"/>
       <c r="D20" s="16"/>
@@ -7078,7 +7043,7 @@
       <c r="BS20" s="20"/>
       <c r="BT20" s="21"/>
     </row>
-    <row r="21" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:72">
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16"/>
@@ -7160,7 +7125,7 @@
       <c r="BS21" s="20"/>
       <c r="BT21" s="21"/>
     </row>
-    <row r="22" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:72">
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
       <c r="D22" s="16"/>
@@ -7242,7 +7207,7 @@
       <c r="BS22" s="20"/>
       <c r="BT22" s="21"/>
     </row>
-    <row r="23" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:72">
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
       <c r="D23" s="16"/>
@@ -7322,7 +7287,7 @@
       <c r="BS23" s="20"/>
       <c r="BT23" s="21"/>
     </row>
-    <row r="24" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:72">
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
       <c r="D24" s="16"/>
@@ -7404,7 +7369,7 @@
       <c r="BS24" s="20"/>
       <c r="BT24" s="21"/>
     </row>
-    <row r="25" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:72">
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
       <c r="D25" s="16"/>
@@ -7480,7 +7445,7 @@
       <c r="BS25" s="20"/>
       <c r="BT25" s="21"/>
     </row>
-    <row r="26" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:72">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="16"/>
@@ -7564,7 +7529,7 @@
       <c r="BS26" s="20"/>
       <c r="BT26" s="21"/>
     </row>
-    <row r="27" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:72">
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
       <c r="D27" s="16"/>
@@ -7648,7 +7613,7 @@
       <c r="BS27" s="20"/>
       <c r="BT27" s="21"/>
     </row>
-    <row r="28" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:72">
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
       <c r="D28" s="16"/>
@@ -7732,7 +7697,7 @@
       <c r="BS28" s="20"/>
       <c r="BT28" s="21"/>
     </row>
-    <row r="29" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:72">
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
       <c r="D29" s="16"/>
@@ -7816,7 +7781,7 @@
       <c r="BS29" s="20"/>
       <c r="BT29" s="21"/>
     </row>
-    <row r="30" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:72">
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
       <c r="D30" s="16"/>
@@ -7896,7 +7861,7 @@
       <c r="BS30" s="20"/>
       <c r="BT30" s="21"/>
     </row>
-    <row r="31" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:72">
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
       <c r="D31" s="16"/>
@@ -7976,7 +7941,7 @@
       <c r="BS31" s="20"/>
       <c r="BT31" s="21"/>
     </row>
-    <row r="32" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:72">
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
       <c r="D32" s="16"/>
@@ -8058,7 +8023,7 @@
       <c r="BS32" s="20"/>
       <c r="BT32" s="21"/>
     </row>
-    <row r="33" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:72">
       <c r="B33" s="14"/>
       <c r="C33" s="15"/>
       <c r="D33" s="16"/>
@@ -8134,7 +8099,7 @@
       <c r="BS33" s="20"/>
       <c r="BT33" s="21"/>
     </row>
-    <row r="34" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:72">
       <c r="B34" s="14"/>
       <c r="C34" s="15"/>
       <c r="D34" s="16"/>
@@ -8214,7 +8179,7 @@
       <c r="BS34" s="20"/>
       <c r="BT34" s="21"/>
     </row>
-    <row r="35" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:72">
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
       <c r="D35" s="16"/>
@@ -8292,7 +8257,7 @@
       <c r="BS35" s="20"/>
       <c r="BT35" s="21"/>
     </row>
-    <row r="36" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:72">
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
       <c r="D36" s="16"/>
@@ -8370,7 +8335,7 @@
       <c r="BS36" s="20"/>
       <c r="BT36" s="21"/>
     </row>
-    <row r="37" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:72">
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
       <c r="D37" s="16"/>
@@ -8448,7 +8413,7 @@
       <c r="BS37" s="20"/>
       <c r="BT37" s="21"/>
     </row>
-    <row r="38" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:72">
       <c r="B38" s="14"/>
       <c r="C38" s="15"/>
       <c r="D38" s="16"/>
@@ -8524,7 +8489,7 @@
       <c r="BS38" s="20"/>
       <c r="BT38" s="21"/>
     </row>
-    <row r="39" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:72">
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
       <c r="D39" s="16"/>
@@ -8600,7 +8565,7 @@
       <c r="BS39" s="20"/>
       <c r="BT39" s="21"/>
     </row>
-    <row r="40" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:72">
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
       <c r="D40" s="16"/>
@@ -8676,7 +8641,7 @@
       <c r="BS40" s="20"/>
       <c r="BT40" s="21"/>
     </row>
-    <row r="41" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:72">
       <c r="B41" s="14"/>
       <c r="C41" s="15"/>
       <c r="D41" s="16"/>
@@ -8760,19 +8725,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:BT42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH34" sqref="AH34"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BO17" sqref="BO17:BO18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6328125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="16384" width="2.6328125" style="1"/>
+    <col min="1" max="16384" width="2.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:72">
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
@@ -8836,7 +8801,7 @@
       <c r="AX2" s="3"/>
       <c r="AY2" s="4"/>
     </row>
-    <row r="3" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:72">
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
@@ -8900,7 +8865,7 @@
       <c r="AX3" s="12"/>
       <c r="AY3" s="13"/>
     </row>
-    <row r="5" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:72">
       <c r="B5" s="22" t="s">
         <v>21</v>
       </c>
@@ -8987,7 +8952,7 @@
       </c>
       <c r="BT5" s="18"/>
     </row>
-    <row r="6" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:72">
       <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
@@ -9037,7 +9002,7 @@
       <c r="BS6" s="20"/>
       <c r="BT6" s="21"/>
     </row>
-    <row r="7" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:72">
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
@@ -9085,7 +9050,7 @@
       <c r="BS7" s="20"/>
       <c r="BT7" s="21"/>
     </row>
-    <row r="8" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:72">
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
@@ -9143,7 +9108,7 @@
       <c r="BS8" s="20"/>
       <c r="BT8" s="21"/>
     </row>
-    <row r="9" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:72">
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
@@ -9226,7 +9191,7 @@
       <c r="BS9" s="20"/>
       <c r="BT9" s="21"/>
     </row>
-    <row r="10" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:72">
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
@@ -9308,7 +9273,7 @@
       <c r="BS10" s="20"/>
       <c r="BT10" s="21"/>
     </row>
-    <row r="11" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:72">
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
@@ -9378,7 +9343,7 @@
       <c r="BS11" s="20"/>
       <c r="BT11" s="21"/>
     </row>
-    <row r="12" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:72">
       <c r="B12" s="14"/>
       <c r="C12" s="15"/>
       <c r="D12" s="16"/>
@@ -9460,7 +9425,7 @@
       <c r="BS12" s="20"/>
       <c r="BT12" s="21"/>
     </row>
-    <row r="13" spans="2:72" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:72" ht="12" customHeight="1">
       <c r="B13" s="14"/>
       <c r="C13" s="15"/>
       <c r="D13" s="16"/>
@@ -9542,7 +9507,7 @@
       <c r="BS13" s="20"/>
       <c r="BT13" s="21"/>
     </row>
-    <row r="14" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:72">
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
@@ -9624,7 +9589,7 @@
       <c r="BS14" s="20"/>
       <c r="BT14" s="21"/>
     </row>
-    <row r="15" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:72">
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
       <c r="D15" s="16"/>
@@ -9693,7 +9658,7 @@
       <c r="BS15" s="20"/>
       <c r="BT15" s="21"/>
     </row>
-    <row r="16" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:72">
       <c r="B16" s="14"/>
       <c r="C16" s="15"/>
       <c r="D16" s="16"/>
@@ -9764,7 +9729,7 @@
       <c r="BS16" s="20"/>
       <c r="BT16" s="21"/>
     </row>
-    <row r="17" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:72">
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
       <c r="D17" s="16"/>
@@ -9834,7 +9799,7 @@
       <c r="BS17" s="20"/>
       <c r="BT17" s="21"/>
     </row>
-    <row r="18" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:72">
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="16"/>
@@ -9916,7 +9881,7 @@
       <c r="BS18" s="20"/>
       <c r="BT18" s="21"/>
     </row>
-    <row r="19" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:72">
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
       <c r="D19" s="16"/>
@@ -10000,7 +9965,7 @@
       <c r="BS19" s="20"/>
       <c r="BT19" s="21"/>
     </row>
-    <row r="20" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:72">
       <c r="B20" s="14"/>
       <c r="C20" s="15"/>
       <c r="D20" s="16"/>
@@ -10082,7 +10047,7 @@
       <c r="BS20" s="20"/>
       <c r="BT20" s="21"/>
     </row>
-    <row r="21" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:72">
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16"/>
@@ -10162,7 +10127,7 @@
       <c r="BS21" s="20"/>
       <c r="BT21" s="21"/>
     </row>
-    <row r="22" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:72">
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
       <c r="D22" s="16"/>
@@ -10242,7 +10207,7 @@
       <c r="BS22" s="20"/>
       <c r="BT22" s="21"/>
     </row>
-    <row r="23" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:72">
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
       <c r="D23" s="16"/>
@@ -10322,7 +10287,7 @@
       <c r="BS23" s="20"/>
       <c r="BT23" s="21"/>
     </row>
-    <row r="24" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:72">
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
       <c r="D24" s="16"/>
@@ -10406,7 +10371,7 @@
       <c r="BS24" s="20"/>
       <c r="BT24" s="21"/>
     </row>
-    <row r="25" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:72">
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
       <c r="D25" s="16"/>
@@ -10490,7 +10455,7 @@
       <c r="BS25" s="20"/>
       <c r="BT25" s="21"/>
     </row>
-    <row r="26" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:72">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="16"/>
@@ -10574,7 +10539,7 @@
       <c r="BS26" s="20"/>
       <c r="BT26" s="21"/>
     </row>
-    <row r="27" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:72">
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
       <c r="D27" s="16"/>
@@ -10658,7 +10623,7 @@
       <c r="BS27" s="20"/>
       <c r="BT27" s="21"/>
     </row>
-    <row r="28" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:72">
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
       <c r="D28" s="16"/>
@@ -10738,7 +10703,7 @@
       <c r="BS28" s="20"/>
       <c r="BT28" s="21"/>
     </row>
-    <row r="29" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:72">
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
       <c r="D29" s="16"/>
@@ -10818,7 +10783,7 @@
       <c r="BS29" s="20"/>
       <c r="BT29" s="21"/>
     </row>
-    <row r="30" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:72">
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
       <c r="D30" s="16"/>
@@ -10900,7 +10865,7 @@
       <c r="BS30" s="20"/>
       <c r="BT30" s="21"/>
     </row>
-    <row r="31" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:72">
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
       <c r="D31" s="16"/>
@@ -10980,7 +10945,7 @@
       <c r="BS31" s="20"/>
       <c r="BT31" s="21"/>
     </row>
-    <row r="32" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:72">
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
       <c r="D32" s="16"/>
@@ -11060,7 +11025,7 @@
       <c r="BS32" s="20"/>
       <c r="BT32" s="21"/>
     </row>
-    <row r="33" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:72">
       <c r="B33" s="14"/>
       <c r="C33" s="15"/>
       <c r="D33" s="16"/>
@@ -11142,7 +11107,7 @@
       <c r="BS33" s="20"/>
       <c r="BT33" s="21"/>
     </row>
-    <row r="34" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:72">
       <c r="B34" s="14"/>
       <c r="C34" s="15"/>
       <c r="D34" s="16"/>
@@ -11224,7 +11189,7 @@
       <c r="BS34" s="20"/>
       <c r="BT34" s="21"/>
     </row>
-    <row r="35" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:72">
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
       <c r="D35" s="16"/>
@@ -11304,7 +11269,7 @@
       <c r="BS35" s="20"/>
       <c r="BT35" s="21"/>
     </row>
-    <row r="36" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:72">
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
       <c r="D36" s="16"/>
@@ -11384,7 +11349,7 @@
       <c r="BS36" s="20"/>
       <c r="BT36" s="21"/>
     </row>
-    <row r="37" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:72">
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
       <c r="D37" s="16"/>
@@ -11464,7 +11429,7 @@
       <c r="BS37" s="20"/>
       <c r="BT37" s="21"/>
     </row>
-    <row r="38" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:72">
       <c r="B38" s="14"/>
       <c r="C38" s="15"/>
       <c r="D38" s="16"/>
@@ -11542,7 +11507,7 @@
       <c r="BS38" s="20"/>
       <c r="BT38" s="21"/>
     </row>
-    <row r="39" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:72">
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
       <c r="D39" s="16"/>
@@ -11620,7 +11585,7 @@
       <c r="BS39" s="20"/>
       <c r="BT39" s="21"/>
     </row>
-    <row r="40" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:72">
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
       <c r="D40" s="16"/>
@@ -11698,7 +11663,7 @@
       <c r="BS40" s="20"/>
       <c r="BT40" s="21"/>
     </row>
-    <row r="41" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:72">
       <c r="B41" s="14"/>
       <c r="C41" s="15"/>
       <c r="D41" s="16"/>
@@ -11776,7 +11741,7 @@
       <c r="BS41" s="20"/>
       <c r="BT41" s="21"/>
     </row>
-    <row r="42" spans="2:72" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:72">
       <c r="R42" s="14" t="s">
         <v>154</v>
       </c>
@@ -11784,19 +11749,19 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11805,12 +11770,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
契約手続き一覧、テストケース Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/テストケース.xlsx
+++ b/テストケース.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="469">
   <si>
     <t>物件管理</t>
     <rPh sb="0" eb="2">
@@ -3419,10 +3419,6 @@
   </si>
   <si>
     <t>進捗情報⑧スケジュール（期日･費用）の設定</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>入金金額、消費税、入金状況、入金日を反映されること。</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -4177,10 +4173,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>可以选择変更後車室番号，与当前车室番号相同的车室不能选择</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">進捗情報①車室変更情報確認 </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -4482,6 +4474,31 @@
   </si>
   <si>
     <t>126</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>鍵類･操作説明書･配置図･保管場所使用承諾証明書送付メールを送信できること。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>入金金額、消費税、入金状況、入金日を反映されること。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>変更可能の項目を変更できること。消費税を自動反映されること。</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヘンコウショルイソウフサキジドウハンエイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>変更後の車室番号が選択できます。しかし、現在の車室と同じ番号の車室が選択できない。</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4831,7 +4848,7 @@
         <xdr:cNvPr id="3" name="図 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6541EA01-6FAB-48A4-A7B7-7B82327644E7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6541EA01-6FAB-48A4-A7B7-7B82327644E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4843,7 +4860,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -4886,7 +4903,7 @@
         <xdr:cNvPr id="3" name="図 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E3E2872-674B-4C30-9DBA-BFEFBCA09095}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E3E2872-674B-4C30-9DBA-BFEFBCA09095}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4898,7 +4915,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -4941,7 +4958,7 @@
         <xdr:cNvPr id="3" name="図 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{92E36B1A-877D-4AEF-B86B-A90F84B8864F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92E36B1A-877D-4AEF-B86B-A90F84B8864F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4953,7 +4970,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -4990,7 +5007,7 @@
         <xdr:cNvPr id="5" name="図 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9DCCE2CA-F9AF-49FA-B913-4029A4E1B2DC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DCCE2CA-F9AF-49FA-B913-4029A4E1B2DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5002,7 +5019,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -5044,7 +5061,7 @@
         <xdr:cNvPr id="3" name="図 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{308EBF97-DA72-41C3-828D-64A4396BEE2E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{308EBF97-DA72-41C3-828D-64A4396BEE2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5056,7 +5073,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -5093,7 +5110,7 @@
         <xdr:cNvPr id="5" name="図 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1D538F92-0C60-4B3C-A99E-ED208ECC5A11}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D538F92-0C60-4B3C-A99E-ED208ECC5A11}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5105,7 +5122,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -14430,8 +14447,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:BU149"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="R97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL116" sqref="AL116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="12"/>
@@ -14675,7 +14692,7 @@
       <c r="S6" s="3"/>
       <c r="T6" s="4"/>
       <c r="U6" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AG6" s="4"/>
       <c r="AH6" s="1" t="s">
@@ -17935,7 +17952,7 @@
       <c r="C59" s="15"/>
       <c r="D59" s="16"/>
       <c r="R59" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="S59" s="15"/>
       <c r="T59" s="16"/>
@@ -18121,7 +18138,7 @@
       <c r="AF64" s="3"/>
       <c r="AG64" s="4"/>
       <c r="AH64" s="2" t="s">
-        <v>324</v>
+        <v>466</v>
       </c>
       <c r="AI64" s="3"/>
       <c r="AJ64" s="3"/>
@@ -18170,14 +18187,14 @@
       <c r="C65" s="15"/>
       <c r="D65" s="16"/>
       <c r="R65" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S65" s="15"/>
       <c r="T65" s="16"/>
       <c r="AF65" s="15"/>
       <c r="AG65" s="16"/>
       <c r="AH65" s="14" t="s">
-        <v>360</v>
+        <v>467</v>
       </c>
       <c r="BO65" s="14" t="str">
         <f t="shared" si="0"/>
@@ -18194,7 +18211,7 @@
       <c r="C66" s="15"/>
       <c r="D66" s="16"/>
       <c r="R66" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="S66" s="15"/>
       <c r="T66" s="16"/>
@@ -18218,12 +18235,12 @@
       <c r="C67" s="15"/>
       <c r="D67" s="16"/>
       <c r="R67" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="S67" s="3"/>
       <c r="T67" s="4"/>
       <c r="U67" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="V67" s="3"/>
       <c r="W67" s="3"/>
@@ -18238,7 +18255,7 @@
       <c r="AF67" s="3"/>
       <c r="AG67" s="4"/>
       <c r="AH67" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AI67" s="3"/>
       <c r="AJ67" s="3"/>
@@ -18287,14 +18304,14 @@
       <c r="C68" s="15"/>
       <c r="D68" s="16"/>
       <c r="R68" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S68" s="15"/>
       <c r="T68" s="16"/>
       <c r="AF68" s="15"/>
       <c r="AG68" s="15"/>
       <c r="AH68" s="14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="BO68" s="14" t="str">
         <f t="shared" si="0"/>
@@ -18311,14 +18328,14 @@
       <c r="C69" s="15"/>
       <c r="D69" s="16"/>
       <c r="R69" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="S69" s="15"/>
       <c r="T69" s="16"/>
       <c r="AF69" s="15"/>
       <c r="AG69" s="16"/>
       <c r="AH69" s="15" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="BO69" s="14" t="str">
         <f t="shared" si="0"/>
@@ -18335,14 +18352,14 @@
       <c r="C70" s="15"/>
       <c r="D70" s="16"/>
       <c r="R70" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="S70" s="15"/>
       <c r="T70" s="16"/>
       <c r="AF70" s="15"/>
       <c r="AG70" s="16"/>
       <c r="AH70" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="BO70" s="14" t="str">
         <f t="shared" si="0"/>
@@ -18359,14 +18376,14 @@
       <c r="C71" s="15"/>
       <c r="D71" s="16"/>
       <c r="R71" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="S71" s="15"/>
       <c r="T71" s="16"/>
       <c r="AF71" s="15"/>
       <c r="AG71" s="16"/>
       <c r="AH71" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="BO71" s="14" t="str">
         <f t="shared" si="0"/>
@@ -18383,14 +18400,14 @@
       <c r="C72" s="15"/>
       <c r="D72" s="16"/>
       <c r="R72" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S72" s="15"/>
       <c r="T72" s="16"/>
       <c r="AF72" s="15"/>
       <c r="AG72" s="16"/>
       <c r="AH72" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="BO72" s="14" t="str">
         <f t="shared" si="0"/>
@@ -18407,14 +18424,14 @@
       <c r="C73" s="15"/>
       <c r="D73" s="16"/>
       <c r="R73" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="S73" s="15"/>
       <c r="T73" s="16"/>
       <c r="AF73" s="15"/>
       <c r="AG73" s="16"/>
       <c r="AH73" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="BO73" s="14" t="str">
         <f t="shared" si="0"/>
@@ -18431,12 +18448,12 @@
       <c r="C74" s="15"/>
       <c r="D74" s="16"/>
       <c r="R74" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="S74" s="3"/>
       <c r="T74" s="4"/>
       <c r="U74" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="V74" s="3"/>
       <c r="W74" s="3"/>
@@ -18451,7 +18468,7 @@
       <c r="AF74" s="3"/>
       <c r="AG74" s="4"/>
       <c r="AH74" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AI74" s="3"/>
       <c r="AJ74" s="3"/>
@@ -18500,12 +18517,12 @@
       <c r="C75" s="15"/>
       <c r="D75" s="16"/>
       <c r="R75" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="S75" s="3"/>
       <c r="T75" s="4"/>
       <c r="U75" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="V75" s="3"/>
       <c r="W75" s="3"/>
@@ -18520,7 +18537,7 @@
       <c r="AF75" s="3"/>
       <c r="AG75" s="4"/>
       <c r="AH75" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AI75" s="3"/>
       <c r="AJ75" s="3"/>
@@ -18569,14 +18586,14 @@
       <c r="C76" s="15"/>
       <c r="D76" s="16"/>
       <c r="R76" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="S76" s="15"/>
       <c r="T76" s="16"/>
       <c r="AF76" s="15"/>
       <c r="AG76" s="16"/>
       <c r="AH76" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="BO76" s="14" t="str">
         <f t="shared" si="0"/>
@@ -18593,12 +18610,12 @@
       <c r="C77" s="15"/>
       <c r="D77" s="16"/>
       <c r="R77" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="S77" s="3"/>
       <c r="T77" s="4"/>
       <c r="U77" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="V77" s="2"/>
       <c r="W77" s="2"/>
@@ -18662,12 +18679,12 @@
       <c r="C78" s="15"/>
       <c r="D78" s="16"/>
       <c r="R78" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="S78" s="3"/>
       <c r="T78" s="4"/>
       <c r="U78" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="V78" s="3"/>
       <c r="W78" s="3"/>
@@ -18682,7 +18699,7 @@
       <c r="AF78" s="3"/>
       <c r="AG78" s="4"/>
       <c r="AH78" s="2" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="AI78" s="3"/>
       <c r="AJ78" s="3"/>
@@ -18731,14 +18748,14 @@
       <c r="C79" s="15"/>
       <c r="D79" s="16"/>
       <c r="R79" s="14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="S79" s="15"/>
       <c r="T79" s="16"/>
       <c r="AF79" s="15"/>
-      <c r="AG79" s="16"/>
+      <c r="AG79" s="15"/>
       <c r="AH79" s="14" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="BO79" s="14" t="str">
         <f t="shared" si="0"/>
@@ -18755,14 +18772,14 @@
       <c r="C80" s="15"/>
       <c r="D80" s="16"/>
       <c r="R80" s="14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="S80" s="15"/>
       <c r="T80" s="16"/>
       <c r="AF80" s="15"/>
       <c r="AG80" s="16"/>
       <c r="AH80" s="1" t="s">
-        <v>347</v>
+        <v>465</v>
       </c>
       <c r="BO80" s="14" t="str">
         <f t="shared" si="0"/>
@@ -18779,12 +18796,12 @@
       <c r="C81" s="15"/>
       <c r="D81" s="16"/>
       <c r="R81" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="S81" s="3"/>
       <c r="T81" s="4"/>
       <c r="U81" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="V81" s="3"/>
       <c r="W81" s="3"/>
@@ -18799,7 +18816,7 @@
       <c r="AF81" s="3"/>
       <c r="AG81" s="4"/>
       <c r="AH81" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AI81" s="3"/>
       <c r="AJ81" s="3"/>
@@ -18848,12 +18865,12 @@
       <c r="C82" s="15"/>
       <c r="D82" s="16"/>
       <c r="R82" s="31" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="S82" s="32"/>
       <c r="T82" s="33"/>
       <c r="U82" s="32" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="V82" s="32"/>
       <c r="W82" s="32"/>
@@ -18868,7 +18885,7 @@
       <c r="AF82" s="32"/>
       <c r="AG82" s="33"/>
       <c r="AH82" s="31" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AI82" s="32"/>
       <c r="AJ82" s="32"/>
@@ -18951,12 +18968,12 @@
       <c r="P84" s="3"/>
       <c r="Q84" s="3"/>
       <c r="R84" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="S84" s="3"/>
       <c r="T84" s="4"/>
       <c r="U84" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="V84" s="3"/>
       <c r="W84" s="3"/>
@@ -18971,7 +18988,7 @@
       <c r="AF84" s="3"/>
       <c r="AG84" s="3"/>
       <c r="AH84" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AI84" s="3"/>
       <c r="AJ84" s="3"/>
@@ -19023,14 +19040,14 @@
         <v>79</v>
       </c>
       <c r="R85" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="S85" s="15"/>
       <c r="T85" s="16"/>
       <c r="AF85" s="15"/>
       <c r="AG85" s="15"/>
       <c r="AH85" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="BO85" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19050,14 +19067,14 @@
         <v>17</v>
       </c>
       <c r="R86" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S86" s="15"/>
       <c r="T86" s="16"/>
       <c r="AF86" s="15"/>
       <c r="AG86" s="15"/>
       <c r="AH86" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="BO86" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19074,15 +19091,15 @@
       <c r="C87" s="15"/>
       <c r="D87" s="16"/>
       <c r="E87" s="14" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="R87" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="S87" s="3"/>
       <c r="T87" s="4"/>
       <c r="U87" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="V87" s="3"/>
       <c r="W87" s="3"/>
@@ -19141,17 +19158,17 @@
       <c r="C88" s="15"/>
       <c r="D88" s="16"/>
       <c r="R88" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="S88" s="15"/>
       <c r="T88" s="16"/>
       <c r="U88" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="AF88" s="15"/>
       <c r="AG88" s="15"/>
       <c r="AH88" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="BO88" s="14" t="str">
         <f t="shared" ref="BO88:BO97" si="1">IF(R88="","",$G$2&amp;"-"&amp;$B$6&amp;"-"&amp;R88)</f>
@@ -19168,7 +19185,7 @@
       <c r="C89" s="15"/>
       <c r="D89" s="16"/>
       <c r="R89" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="S89" s="15"/>
       <c r="T89" s="16"/>
@@ -19192,14 +19209,14 @@
       <c r="C90" s="15"/>
       <c r="D90" s="16"/>
       <c r="R90" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="S90" s="15"/>
       <c r="T90" s="16"/>
       <c r="AF90" s="15"/>
       <c r="AG90" s="16"/>
       <c r="AH90" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="BO90" s="14" t="str">
         <f t="shared" si="1"/>
@@ -19216,14 +19233,14 @@
       <c r="C91" s="15"/>
       <c r="D91" s="16"/>
       <c r="R91" s="14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="S91" s="15"/>
       <c r="T91" s="16"/>
       <c r="AF91" s="15"/>
       <c r="AG91" s="16"/>
       <c r="AH91" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="BO91" s="14" t="str">
         <f t="shared" si="1"/>
@@ -19240,14 +19257,14 @@
       <c r="C92" s="15"/>
       <c r="D92" s="16"/>
       <c r="R92" s="14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="S92" s="15"/>
       <c r="T92" s="16"/>
       <c r="AF92" s="15"/>
       <c r="AG92" s="16"/>
       <c r="AH92" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="BO92" s="14" t="str">
         <f t="shared" si="1"/>
@@ -19264,14 +19281,14 @@
       <c r="C93" s="15"/>
       <c r="D93" s="16"/>
       <c r="R93" s="14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="S93" s="15"/>
       <c r="T93" s="16"/>
       <c r="AF93" s="15"/>
       <c r="AG93" s="16"/>
       <c r="AH93" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="BO93" s="14" t="str">
         <f t="shared" si="1"/>
@@ -19288,12 +19305,12 @@
       <c r="C94" s="15"/>
       <c r="D94" s="16"/>
       <c r="R94" s="14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="S94" s="15"/>
       <c r="T94" s="15"/>
       <c r="U94" s="14" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="V94" s="15"/>
       <c r="W94" s="15"/>
@@ -19308,7 +19325,7 @@
       <c r="AF94" s="15"/>
       <c r="AG94" s="15"/>
       <c r="AH94" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AI94" s="15"/>
       <c r="AJ94" s="15"/>
@@ -19357,17 +19374,17 @@
       <c r="C95" s="15"/>
       <c r="D95" s="16"/>
       <c r="R95" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="S95" s="15"/>
       <c r="T95" s="16"/>
       <c r="U95" s="15" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="AF95" s="15"/>
       <c r="AG95" s="16"/>
       <c r="AH95" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="BO95" s="14" t="str">
         <f t="shared" si="1"/>
@@ -19384,7 +19401,7 @@
       <c r="C96" s="15"/>
       <c r="D96" s="16"/>
       <c r="R96" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="S96" s="15"/>
       <c r="T96" s="16"/>
@@ -19409,14 +19426,14 @@
       <c r="C97" s="15"/>
       <c r="D97" s="16"/>
       <c r="R97" s="14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="S97" s="15"/>
       <c r="T97" s="16"/>
       <c r="AF97" s="15"/>
       <c r="AG97" s="16"/>
       <c r="AH97" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="BO97" s="26" t="str">
         <f t="shared" si="1"/>
@@ -19436,7 +19453,7 @@
       <c r="S98" s="3"/>
       <c r="T98" s="4"/>
       <c r="U98" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="V98" s="3"/>
       <c r="W98" s="3"/>
@@ -19498,17 +19515,17 @@
       <c r="C99" s="15"/>
       <c r="D99" s="16"/>
       <c r="R99" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="S99" s="15"/>
       <c r="T99" s="16"/>
       <c r="U99" s="15" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AF99" s="15"/>
       <c r="AG99" s="16"/>
       <c r="AH99" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="BO99" s="14" t="str">
         <f t="shared" si="2"/>
@@ -19525,17 +19542,17 @@
       <c r="C100" s="15"/>
       <c r="D100" s="16"/>
       <c r="R100" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="S100" s="15"/>
       <c r="T100" s="16"/>
       <c r="U100" s="15" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="AF100" s="15"/>
       <c r="AG100" s="16"/>
       <c r="AH100" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="BO100" s="14" t="str">
         <f t="shared" si="2"/>
@@ -19552,7 +19569,7 @@
       <c r="C101" s="15"/>
       <c r="D101" s="16"/>
       <c r="R101" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="S101" s="15"/>
       <c r="T101" s="16"/>
@@ -19577,7 +19594,7 @@
       <c r="C102" s="15"/>
       <c r="D102" s="16"/>
       <c r="R102" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="S102" s="15"/>
       <c r="T102" s="16"/>
@@ -19585,7 +19602,7 @@
       <c r="AF102" s="15"/>
       <c r="AG102" s="16"/>
       <c r="AH102" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="BO102" s="26" t="str">
         <f t="shared" si="2"/>
@@ -19605,7 +19622,7 @@
       <c r="S103" s="3"/>
       <c r="T103" s="4"/>
       <c r="U103" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="V103" s="3"/>
       <c r="W103" s="3"/>
@@ -19667,12 +19684,12 @@
       <c r="C104" s="15"/>
       <c r="D104" s="16"/>
       <c r="R104" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="S104" s="15"/>
       <c r="T104" s="16"/>
       <c r="U104" s="15" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="AF104" s="15"/>
       <c r="AG104" s="16"/>
@@ -19694,12 +19711,12 @@
       <c r="C105" s="15"/>
       <c r="D105" s="16"/>
       <c r="R105" s="14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S105" s="15"/>
       <c r="T105" s="16"/>
       <c r="U105" s="15" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="AF105" s="15"/>
       <c r="AG105" s="16"/>
@@ -19717,12 +19734,12 @@
       <c r="B106" s="14"/>
       <c r="E106" s="14"/>
       <c r="R106" s="14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="S106" s="15"/>
       <c r="T106" s="16"/>
       <c r="U106" s="15" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="AF106" s="15"/>
       <c r="AG106" s="16"/>
@@ -19740,15 +19757,15 @@
       <c r="B107" s="14"/>
       <c r="E107" s="14"/>
       <c r="R107" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="S107" s="15"/>
       <c r="T107" s="16"/>
       <c r="U107" s="15" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="AH107" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="BO107" s="14" t="str">
         <f t="shared" si="2"/>
@@ -19764,7 +19781,7 @@
       <c r="B108" s="14"/>
       <c r="E108" s="14"/>
       <c r="R108" s="14" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="S108" s="15"/>
       <c r="T108" s="16"/>
@@ -19786,13 +19803,13 @@
       <c r="B109" s="14"/>
       <c r="E109" s="14"/>
       <c r="R109" s="14" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="S109" s="15"/>
       <c r="T109" s="16"/>
       <c r="U109" s="15"/>
       <c r="AH109" s="26" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="BO109" s="26" t="str">
         <f t="shared" si="2"/>
@@ -19808,7 +19825,7 @@
       <c r="B110" s="14"/>
       <c r="E110" s="14"/>
       <c r="R110" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="S110" s="3"/>
       <c r="T110" s="4"/>
@@ -19828,7 +19845,7 @@
       <c r="AF110" s="3"/>
       <c r="AG110" s="3"/>
       <c r="AH110" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="AI110" s="3"/>
       <c r="AJ110" s="3"/>
@@ -19890,7 +19907,7 @@
       <c r="P111" s="27"/>
       <c r="Q111" s="28"/>
       <c r="R111" s="31" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="S111" s="32"/>
       <c r="T111" s="33"/>
@@ -19910,7 +19927,7 @@
       <c r="AF111" s="32"/>
       <c r="AG111" s="32"/>
       <c r="AH111" s="31" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AI111" s="32"/>
       <c r="AJ111" s="32"/>
@@ -19960,15 +19977,15 @@
         <v>18</v>
       </c>
       <c r="R112" s="14" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="S112" s="15"/>
       <c r="T112" s="16"/>
       <c r="U112" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AH112" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="BO112" s="14" t="str">
         <f t="shared" si="2"/>
@@ -19986,12 +20003,12 @@
         <v>79</v>
       </c>
       <c r="R113" s="14" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S113" s="15"/>
       <c r="T113" s="16"/>
       <c r="AH113" s="14" t="s">
-        <v>405</v>
+        <v>468</v>
       </c>
       <c r="BO113" s="14" t="str">
         <f t="shared" si="2"/>
@@ -20009,7 +20026,7 @@
         <v>17</v>
       </c>
       <c r="R114" s="26" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="S114" s="27"/>
       <c r="T114" s="28"/>
@@ -20027,7 +20044,7 @@
       <c r="AF114" s="27"/>
       <c r="AG114" s="27"/>
       <c r="AH114" s="26" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AI114" s="27"/>
       <c r="AJ114" s="27"/>
@@ -20074,19 +20091,19 @@
     <row r="115" spans="2:73">
       <c r="B115" s="14"/>
       <c r="E115" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="R115" s="14" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="S115" s="15"/>
       <c r="T115" s="16"/>
       <c r="U115" s="15" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="V115" s="15"/>
       <c r="AH115" s="39" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="BO115" s="14" t="str">
         <f t="shared" si="2"/>
@@ -20102,12 +20119,12 @@
       <c r="B116" s="14"/>
       <c r="E116" s="14"/>
       <c r="R116" s="14" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="S116" s="15"/>
       <c r="T116" s="16"/>
       <c r="U116" s="15" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="V116" s="15"/>
       <c r="AH116" s="14" t="s">
@@ -20127,14 +20144,14 @@
       <c r="B117" s="14"/>
       <c r="E117" s="14"/>
       <c r="R117" s="14" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="S117" s="15"/>
       <c r="T117" s="16"/>
       <c r="U117" s="15"/>
       <c r="V117" s="15"/>
       <c r="AH117" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BO117" s="14" t="str">
         <f t="shared" si="2"/>
@@ -20151,7 +20168,7 @@
       <c r="B118" s="14"/>
       <c r="E118" s="14"/>
       <c r="R118" s="14" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S118" s="15"/>
       <c r="T118" s="16"/>
@@ -20175,16 +20192,16 @@
       <c r="B119" s="14"/>
       <c r="E119" s="14"/>
       <c r="R119" s="14" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S119" s="15"/>
       <c r="T119" s="16"/>
       <c r="U119" s="15" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="V119" s="15"/>
       <c r="AH119" s="14" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="BO119" s="14" t="str">
         <f t="shared" si="2"/>
@@ -20199,7 +20216,7 @@
       <c r="B120" s="14"/>
       <c r="E120" s="14"/>
       <c r="R120" s="14" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="S120" s="15"/>
       <c r="T120" s="16"/>
@@ -20221,14 +20238,14 @@
       <c r="B121" s="14"/>
       <c r="E121" s="14"/>
       <c r="R121" s="14" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="S121" s="15"/>
       <c r="T121" s="16"/>
       <c r="U121" s="15"/>
       <c r="V121" s="15"/>
       <c r="AH121" s="14" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="BO121" s="14" t="str">
         <f t="shared" si="2"/>
@@ -20243,14 +20260,14 @@
       <c r="B122" s="14"/>
       <c r="E122" s="14"/>
       <c r="R122" s="14" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="S122" s="15"/>
       <c r="T122" s="16"/>
       <c r="U122" s="15"/>
       <c r="V122" s="15"/>
       <c r="AH122" s="14" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="BO122" s="14" t="str">
         <f t="shared" si="2"/>
@@ -20265,14 +20282,14 @@
       <c r="B123" s="14"/>
       <c r="E123" s="14"/>
       <c r="R123" s="14" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="S123" s="15"/>
       <c r="T123" s="16"/>
       <c r="U123" s="15"/>
       <c r="V123" s="15"/>
       <c r="AH123" s="14" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="BO123" s="14" t="str">
         <f t="shared" si="2"/>
@@ -20287,14 +20304,14 @@
       <c r="B124" s="14"/>
       <c r="E124" s="14"/>
       <c r="R124" s="14" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="S124" s="15"/>
       <c r="T124" s="16"/>
       <c r="U124" s="15"/>
       <c r="V124" s="15"/>
       <c r="AH124" s="14" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="BO124" s="14" t="str">
         <f t="shared" si="2"/>
@@ -20309,7 +20326,7 @@
       <c r="B125" s="14"/>
       <c r="E125" s="14"/>
       <c r="R125" s="14" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="S125" s="15"/>
       <c r="T125" s="16"/>
@@ -20331,16 +20348,16 @@
       <c r="B126" s="14"/>
       <c r="E126" s="14"/>
       <c r="R126" s="14" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="S126" s="15"/>
       <c r="T126" s="16"/>
       <c r="U126" s="15" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="V126" s="15"/>
       <c r="AH126" s="38" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="BO126" s="14" t="str">
         <f t="shared" si="2"/>
@@ -20355,14 +20372,14 @@
       <c r="B127" s="14"/>
       <c r="E127" s="14"/>
       <c r="R127" s="14" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="S127" s="15"/>
       <c r="T127" s="16"/>
       <c r="U127" s="15"/>
       <c r="V127" s="15"/>
       <c r="AH127" s="14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="BO127" s="14" t="str">
         <f t="shared" si="2"/>
@@ -20377,7 +20394,7 @@
       <c r="B128" s="14"/>
       <c r="E128" s="14"/>
       <c r="R128" s="14" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="S128" s="15"/>
       <c r="T128" s="16"/>
@@ -20399,14 +20416,14 @@
       <c r="B129" s="14"/>
       <c r="E129" s="14"/>
       <c r="R129" s="14" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="S129" s="15"/>
       <c r="T129" s="16"/>
       <c r="U129" s="15"/>
       <c r="V129" s="15"/>
       <c r="AH129" s="14" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="BO129" s="14" t="str">
         <f t="shared" si="2"/>
@@ -20421,12 +20438,12 @@
       <c r="B130" s="14"/>
       <c r="E130" s="14"/>
       <c r="R130" s="14" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="S130" s="15"/>
       <c r="T130" s="16"/>
       <c r="U130" s="15" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="V130" s="15"/>
       <c r="AH130" s="14" t="s">
@@ -20445,12 +20462,12 @@
       <c r="B131" s="14"/>
       <c r="E131" s="14"/>
       <c r="R131" s="14" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="S131" s="15"/>
       <c r="T131" s="16"/>
       <c r="U131" s="15" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="V131" s="15"/>
       <c r="AH131" s="14" t="s">
@@ -20469,7 +20486,7 @@
       <c r="B132" s="14"/>
       <c r="E132" s="14"/>
       <c r="R132" s="14" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="S132" s="15"/>
       <c r="T132" s="16"/>
@@ -20491,14 +20508,14 @@
       <c r="B133" s="14"/>
       <c r="E133" s="14"/>
       <c r="R133" s="14" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="S133" s="15"/>
       <c r="T133" s="16"/>
       <c r="U133" s="15"/>
       <c r="V133" s="15"/>
       <c r="AH133" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="BO133" s="14" t="str">
         <f t="shared" si="2"/>
@@ -20513,12 +20530,12 @@
       <c r="B134" s="14"/>
       <c r="E134" s="14"/>
       <c r="R134" s="14" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="S134" s="15"/>
       <c r="T134" s="16"/>
       <c r="U134" s="15" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="V134" s="15"/>
       <c r="AH134" s="14"/>
@@ -20535,7 +20552,7 @@
       <c r="B135" s="14"/>
       <c r="E135" s="14"/>
       <c r="R135" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="S135" s="3"/>
       <c r="T135" s="4"/>
@@ -20555,7 +20572,7 @@
       <c r="AF135" s="3"/>
       <c r="AG135" s="3"/>
       <c r="AH135" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="AI135" s="3"/>
       <c r="AJ135" s="3"/>
@@ -20616,7 +20633,7 @@
       <c r="P136" s="27"/>
       <c r="Q136" s="28"/>
       <c r="R136" s="31" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="S136" s="32"/>
       <c r="T136" s="33"/>
@@ -20636,7 +20653,7 @@
       <c r="AF136" s="32"/>
       <c r="AG136" s="32"/>
       <c r="AH136" s="31" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AI136" s="32"/>
       <c r="AJ136" s="32"/>

</xml_diff>